<commit_message>
Renamed folder updated comaprison
</commit_message>
<xml_diff>
--- a/Comparision.xlsx
+++ b/Comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/dev/uni/vision/AISSCV_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AA9C25-B31F-4D4E-85C7-86EBBDB8440B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805A5E7A-33F2-1340-BC53-CB92225120A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16420" yWindow="2940" windowWidth="43740" windowHeight="29460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16420" yWindow="2940" windowWidth="43740" windowHeight="29460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Class" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="88">
   <si>
     <t>run</t>
   </si>
@@ -251,12 +251,6 @@
     <t>Adding Occlution (Cutout)</t>
   </si>
   <si>
-    <t>occlution p=0.75, max size=0.4</t>
-  </si>
-  <si>
-    <t>occlution p=0.5, max size=0.35</t>
-  </si>
-  <si>
     <t>unlabeld data</t>
   </si>
   <si>
@@ -285,6 +279,24 @@
   </si>
   <si>
     <t>3000 (basis)</t>
+  </si>
+  <si>
+    <t>Basis (Color, Batch Size 3000, 10 Augmentations)</t>
+  </si>
+  <si>
+    <t>occlution p=0,75, max size=0,4</t>
+  </si>
+  <si>
+    <t>occlution p=0,5, max size=0,35</t>
+  </si>
+  <si>
+    <t>No Label, Occlution (0,5/0,35), Batch Size 3500</t>
+  </si>
+  <si>
+    <t>Color (10 fold)</t>
+  </si>
+  <si>
+    <t>No Label, Occlude 50% smaller size, batch size 3500 (10 fold)</t>
   </si>
 </sst>
 </file>
@@ -736,7 +748,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -915,6 +927,9 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -926,15 +941,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -948,38 +954,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="100">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="98">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2263,8 +2262,8 @@
   </sheetPr>
   <dimension ref="A1:L221"/>
   <sheetViews>
-    <sheetView zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
-      <selection activeCell="D232" sqref="D232"/>
+    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
+      <selection activeCell="G231" sqref="G231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2278,18 +2277,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="98" t="s">
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -2887,18 +2886,18 @@
       <c r="J18" s="56"/>
     </row>
     <row r="20" spans="1:12" ht="26" x14ac:dyDescent="0.2">
-      <c r="A20" s="98" t="s">
+      <c r="A20" s="99" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="98"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="98" t="s">
+      <c r="B20" s="99"/>
+      <c r="C20" s="99"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="98"/>
-      <c r="G20" s="98"/>
-      <c r="H20" s="98"/>
+      <c r="F20" s="99"/>
+      <c r="G20" s="99"/>
+      <c r="H20" s="99"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
@@ -3496,18 +3495,18 @@
       <c r="J37" s="56"/>
     </row>
     <row r="39" spans="1:12" ht="26" x14ac:dyDescent="0.2">
-      <c r="A39" s="98" t="s">
+      <c r="A39" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="98"/>
-      <c r="C39" s="98"/>
-      <c r="D39" s="99"/>
-      <c r="E39" s="98" t="s">
+      <c r="B39" s="99"/>
+      <c r="C39" s="99"/>
+      <c r="D39" s="100"/>
+      <c r="E39" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="F39" s="98"/>
-      <c r="G39" s="98"/>
-      <c r="H39" s="98"/>
+      <c r="F39" s="99"/>
+      <c r="G39" s="99"/>
+      <c r="H39" s="99"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
@@ -4101,18 +4100,18 @@
       </c>
     </row>
     <row r="56" spans="1:12" ht="26" x14ac:dyDescent="0.2">
-      <c r="A56" s="98" t="s">
+      <c r="A56" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="98"/>
-      <c r="C56" s="98"/>
-      <c r="D56" s="99"/>
-      <c r="E56" s="98" t="s">
+      <c r="B56" s="99"/>
+      <c r="C56" s="99"/>
+      <c r="D56" s="100"/>
+      <c r="E56" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="F56" s="98"/>
-      <c r="G56" s="98"/>
-      <c r="H56" s="98"/>
+      <c r="F56" s="99"/>
+      <c r="G56" s="99"/>
+      <c r="H56" s="99"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
@@ -4706,18 +4705,18 @@
       </c>
     </row>
     <row r="75" spans="1:12" ht="26" x14ac:dyDescent="0.2">
-      <c r="A75" s="98" t="s">
+      <c r="A75" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="B75" s="98"/>
-      <c r="C75" s="98"/>
-      <c r="D75" s="99"/>
-      <c r="E75" s="98" t="s">
+      <c r="B75" s="99"/>
+      <c r="C75" s="99"/>
+      <c r="D75" s="100"/>
+      <c r="E75" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="F75" s="98"/>
-      <c r="G75" s="98"/>
-      <c r="H75" s="98"/>
+      <c r="F75" s="99"/>
+      <c r="G75" s="99"/>
+      <c r="H75" s="99"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
@@ -5311,18 +5310,18 @@
       </c>
     </row>
     <row r="96" spans="1:12" ht="26" x14ac:dyDescent="0.2">
-      <c r="A96" s="98" t="s">
+      <c r="A96" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="B96" s="98"/>
-      <c r="C96" s="98"/>
-      <c r="D96" s="99"/>
-      <c r="E96" s="98" t="s">
+      <c r="B96" s="99"/>
+      <c r="C96" s="99"/>
+      <c r="D96" s="100"/>
+      <c r="E96" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="F96" s="98"/>
-      <c r="G96" s="98"/>
-      <c r="H96" s="98"/>
+      <c r="F96" s="99"/>
+      <c r="G96" s="99"/>
+      <c r="H96" s="99"/>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
@@ -5916,18 +5915,18 @@
       </c>
     </row>
     <row r="114" spans="1:12" ht="26" x14ac:dyDescent="0.2">
-      <c r="A114" s="98" t="s">
+      <c r="A114" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="B114" s="98"/>
-      <c r="C114" s="98"/>
-      <c r="D114" s="99"/>
-      <c r="E114" s="98" t="s">
+      <c r="B114" s="99"/>
+      <c r="C114" s="99"/>
+      <c r="D114" s="100"/>
+      <c r="E114" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="F114" s="98"/>
-      <c r="G114" s="98"/>
-      <c r="H114" s="98"/>
+      <c r="F114" s="99"/>
+      <c r="G114" s="99"/>
+      <c r="H114" s="99"/>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
@@ -6525,18 +6524,18 @@
       </c>
     </row>
     <row r="132" spans="1:12" ht="26" x14ac:dyDescent="0.2">
-      <c r="A132" s="98" t="s">
+      <c r="A132" s="99" t="s">
         <v>51</v>
       </c>
-      <c r="B132" s="98"/>
-      <c r="C132" s="98"/>
-      <c r="D132" s="99"/>
-      <c r="E132" s="98" t="s">
+      <c r="B132" s="99"/>
+      <c r="C132" s="99"/>
+      <c r="D132" s="100"/>
+      <c r="E132" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="F132" s="98"/>
-      <c r="G132" s="98"/>
-      <c r="H132" s="98"/>
+      <c r="F132" s="99"/>
+      <c r="G132" s="99"/>
+      <c r="H132" s="99"/>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" s="44" t="s">
@@ -7130,18 +7129,18 @@
       </c>
     </row>
     <row r="151" spans="1:12" ht="26" x14ac:dyDescent="0.2">
-      <c r="A151" s="98" t="s">
+      <c r="A151" s="99" t="s">
         <v>53</v>
       </c>
-      <c r="B151" s="98"/>
-      <c r="C151" s="98"/>
-      <c r="D151" s="99"/>
-      <c r="E151" s="98" t="s">
+      <c r="B151" s="99"/>
+      <c r="C151" s="99"/>
+      <c r="D151" s="100"/>
+      <c r="E151" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="F151" s="98"/>
-      <c r="G151" s="98"/>
-      <c r="H151" s="98"/>
+      <c r="F151" s="99"/>
+      <c r="G151" s="99"/>
+      <c r="H151" s="99"/>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
@@ -7735,18 +7734,18 @@
       </c>
     </row>
     <row r="169" spans="1:12" ht="26" x14ac:dyDescent="0.2">
-      <c r="A169" s="98" t="s">
+      <c r="A169" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="B169" s="98"/>
-      <c r="C169" s="98"/>
-      <c r="D169" s="99"/>
-      <c r="E169" s="98" t="s">
+      <c r="B169" s="99"/>
+      <c r="C169" s="99"/>
+      <c r="D169" s="100"/>
+      <c r="E169" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="F169" s="98"/>
-      <c r="G169" s="98"/>
-      <c r="H169" s="98"/>
+      <c r="F169" s="99"/>
+      <c r="G169" s="99"/>
+      <c r="H169" s="99"/>
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A170" s="59" t="s">
@@ -8340,18 +8339,18 @@
       </c>
     </row>
     <row r="187" spans="1:12" ht="26" x14ac:dyDescent="0.2">
-      <c r="A187" s="98" t="s">
+      <c r="A187" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="B187" s="98"/>
-      <c r="C187" s="98"/>
-      <c r="D187" s="99"/>
-      <c r="E187" s="98" t="s">
+      <c r="B187" s="99"/>
+      <c r="C187" s="99"/>
+      <c r="D187" s="100"/>
+      <c r="E187" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="F187" s="98"/>
-      <c r="G187" s="98"/>
-      <c r="H187" s="98"/>
+      <c r="F187" s="99"/>
+      <c r="G187" s="99"/>
+      <c r="H187" s="99"/>
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
@@ -8945,18 +8944,18 @@
       </c>
     </row>
     <row r="205" spans="1:12" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A205" s="100" t="s">
-        <v>63</v>
-      </c>
-      <c r="B205" s="100"/>
-      <c r="C205" s="100"/>
-      <c r="D205" s="101"/>
-      <c r="E205" s="98" t="s">
-        <v>38</v>
-      </c>
-      <c r="F205" s="98"/>
-      <c r="G205" s="98"/>
-      <c r="H205" s="98"/>
+      <c r="A205" s="101" t="s">
+        <v>87</v>
+      </c>
+      <c r="B205" s="101"/>
+      <c r="C205" s="101"/>
+      <c r="D205" s="102"/>
+      <c r="E205" s="99" t="s">
+        <v>86</v>
+      </c>
+      <c r="F205" s="99"/>
+      <c r="G205" s="99"/>
+      <c r="H205" s="99"/>
     </row>
     <row r="206" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
@@ -9011,26 +9010,26 @@
         <v>18</v>
       </c>
       <c r="F207" s="51">
-        <v>0.93066000000000015</v>
+        <v>0.93520000000000003</v>
       </c>
       <c r="G207">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H207">
-        <v>6</v>
+        <v>2.8</v>
       </c>
       <c r="I207" s="57"/>
       <c r="J207" s="51">
         <f t="shared" ref="J207:J220" si="33">B207-F207</f>
-        <v>-3.8700000000000401E-3</v>
+        <v>-8.4099999999999175E-3</v>
       </c>
       <c r="K207">
         <f t="shared" ref="K207:K220" si="34">C207-G207</f>
-        <v>-6.9</v>
+        <v>9.9999999999999645E-2</v>
       </c>
       <c r="L207">
         <f t="shared" ref="L207:L220" si="35">D207-H207</f>
-        <v>-3.6</v>
+        <v>-0.39999999999999991</v>
       </c>
     </row>
     <row r="208" spans="1:12" x14ac:dyDescent="0.2">
@@ -9050,26 +9049,26 @@
         <v>21</v>
       </c>
       <c r="F208" s="51">
-        <v>0.82050000000000001</v>
+        <v>0.7904500000000001</v>
       </c>
       <c r="G208">
-        <v>22.8</v>
+        <v>11.1</v>
       </c>
       <c r="H208">
-        <v>4.4000000000000004</v>
+        <v>3</v>
       </c>
       <c r="I208" s="57"/>
       <c r="J208" s="51">
         <f t="shared" si="33"/>
-        <v>-8.3900000000000086E-3</v>
+        <v>2.1659999999999902E-2</v>
       </c>
       <c r="K208">
         <f t="shared" si="34"/>
-        <v>-11.600000000000001</v>
+        <v>9.9999999999999645E-2</v>
       </c>
       <c r="L208">
         <f t="shared" si="35"/>
-        <v>-1.6000000000000005</v>
+        <v>-0.20000000000000018</v>
       </c>
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.2">
@@ -9089,26 +9088,26 @@
         <v>19</v>
       </c>
       <c r="F209" s="51">
-        <v>0.79600000000000004</v>
+        <v>0.81349000000000005</v>
       </c>
       <c r="G209">
-        <v>10.6</v>
+        <v>5.3</v>
       </c>
       <c r="H209">
-        <v>4.2</v>
+        <v>2.9</v>
       </c>
       <c r="I209" s="57"/>
       <c r="J209" s="51">
         <f t="shared" si="33"/>
-        <v>4.6669999999999989E-2</v>
+        <v>2.9179999999999984E-2</v>
       </c>
       <c r="K209">
         <f t="shared" si="34"/>
-        <v>-5</v>
+        <v>0.29999999999999982</v>
       </c>
       <c r="L209">
         <f t="shared" si="35"/>
-        <v>-1.6</v>
+        <v>-0.29999999999999982</v>
       </c>
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.2">
@@ -9128,26 +9127,26 @@
         <v>30</v>
       </c>
       <c r="F210" s="51">
-        <v>0.99393999999999993</v>
+        <v>0.99666999999999994</v>
       </c>
       <c r="G210">
-        <v>10.4</v>
+        <v>5.2</v>
       </c>
       <c r="H210">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="I210" s="57"/>
       <c r="J210" s="51">
         <f t="shared" si="33"/>
-        <v>3.500000000001835E-4</v>
+        <v>-2.3799999999998267E-3</v>
       </c>
       <c r="K210">
         <f t="shared" si="34"/>
-        <v>-5.2</v>
+        <v>0</v>
       </c>
       <c r="L210">
         <f t="shared" si="35"/>
-        <v>-0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="211" spans="1:12" x14ac:dyDescent="0.2">
@@ -9167,26 +9166,26 @@
         <v>25</v>
       </c>
       <c r="F211" s="51">
-        <v>0.95017999999999991</v>
+        <v>0.97725000000000006</v>
       </c>
       <c r="G211">
-        <v>13</v>
+        <v>6.7</v>
       </c>
       <c r="H211">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="I211" s="57"/>
       <c r="J211" s="51">
         <f t="shared" si="33"/>
-        <v>3.803000000000023E-2</v>
+        <v>1.0960000000000081E-2</v>
       </c>
       <c r="K211">
         <f t="shared" si="34"/>
-        <v>-6.3</v>
+        <v>0</v>
       </c>
       <c r="L211">
         <f t="shared" si="35"/>
-        <v>-0.8</v>
+        <v>-9.9999999999999978E-2</v>
       </c>
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.2">
@@ -9206,26 +9205,26 @@
         <v>27</v>
       </c>
       <c r="F212" s="51">
-        <v>0.83878000000000008</v>
+        <v>0.86822999999999995</v>
       </c>
       <c r="G212">
-        <v>20</v>
+        <v>10.6</v>
       </c>
       <c r="H212">
-        <v>6.8</v>
+        <v>2.1</v>
       </c>
       <c r="I212" s="57"/>
       <c r="J212" s="51">
         <f t="shared" si="33"/>
-        <v>3.3199999999999896E-3</v>
+        <v>-2.6129999999999876E-2</v>
       </c>
       <c r="K212">
         <f t="shared" si="34"/>
-        <v>-9.4</v>
+        <v>0</v>
       </c>
       <c r="L212">
         <f t="shared" si="35"/>
-        <v>-4.4000000000000004</v>
+        <v>0.29999999999999982</v>
       </c>
     </row>
     <row r="213" spans="1:12" x14ac:dyDescent="0.2">
@@ -9245,26 +9244,26 @@
         <v>28</v>
       </c>
       <c r="F213" s="51">
-        <v>0.90058000000000005</v>
+        <v>0.91077000000000008</v>
       </c>
       <c r="G213">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H213">
-        <v>1.2</v>
+        <v>0.7</v>
       </c>
       <c r="I213" s="57"/>
       <c r="J213" s="51">
         <f t="shared" si="33"/>
-        <v>4.2999999999999705E-3</v>
+        <v>-5.8900000000000619E-3</v>
       </c>
       <c r="K213">
         <f t="shared" si="34"/>
-        <v>-5.9</v>
+        <v>9.9999999999999645E-2</v>
       </c>
       <c r="L213">
         <f t="shared" si="35"/>
-        <v>-0.7</v>
+        <v>-0.19999999999999996</v>
       </c>
     </row>
     <row r="214" spans="1:12" x14ac:dyDescent="0.2">
@@ -9284,26 +9283,26 @@
         <v>23</v>
       </c>
       <c r="F214" s="51">
-        <v>0.96264000000000005</v>
+        <v>0.97732999999999992</v>
       </c>
       <c r="G214">
-        <v>14.8</v>
+        <v>7.5</v>
       </c>
       <c r="H214">
-        <v>4.5999999999999996</v>
+        <v>2.5</v>
       </c>
       <c r="I214" s="57"/>
       <c r="J214" s="51">
         <f t="shared" si="33"/>
-        <v>2.1240000000000037E-2</v>
+        <v>6.5500000000001668E-3</v>
       </c>
       <c r="K214">
         <f t="shared" si="34"/>
-        <v>-7.4</v>
+        <v>-9.9999999999999645E-2</v>
       </c>
       <c r="L214">
         <f t="shared" si="35"/>
-        <v>-2.0999999999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:12" x14ac:dyDescent="0.2">
@@ -9323,26 +9322,26 @@
         <v>24</v>
       </c>
       <c r="F215" s="51">
-        <v>0.94891999999999999</v>
+        <v>0.95444999999999991</v>
       </c>
       <c r="G215">
-        <v>10.6</v>
+        <v>5.4</v>
       </c>
       <c r="H215">
-        <v>4.5999999999999996</v>
+        <v>2.5</v>
       </c>
       <c r="I215" s="57"/>
       <c r="J215" s="51">
         <f t="shared" si="33"/>
-        <v>1.2080000000000091E-2</v>
+        <v>6.5500000000001668E-3</v>
       </c>
       <c r="K215">
         <f t="shared" si="34"/>
-        <v>-5.0999999999999996</v>
+        <v>9.9999999999999645E-2</v>
       </c>
       <c r="L215">
         <f t="shared" si="35"/>
-        <v>-2.0999999999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216" spans="1:12" x14ac:dyDescent="0.2">
@@ -9362,26 +9361,26 @@
         <v>17</v>
       </c>
       <c r="F216" s="51">
-        <v>0.75853999999999999</v>
+        <v>0.79961000000000004</v>
       </c>
       <c r="G216">
-        <v>21</v>
+        <v>10.7</v>
       </c>
       <c r="H216">
-        <v>10</v>
+        <v>4.7</v>
       </c>
       <c r="I216" s="57"/>
       <c r="J216" s="51">
         <f t="shared" si="33"/>
-        <v>4.4100000000000028E-2</v>
+        <v>3.0299999999999772E-3</v>
       </c>
       <c r="K216">
         <f t="shared" si="34"/>
-        <v>-10.3</v>
+        <v>0</v>
       </c>
       <c r="L216">
         <f t="shared" si="35"/>
-        <v>-5.9</v>
+        <v>-0.60000000000000053</v>
       </c>
     </row>
     <row r="217" spans="1:12" x14ac:dyDescent="0.2">
@@ -9401,26 +9400,26 @@
         <v>20</v>
       </c>
       <c r="F217" s="51">
-        <v>0.78142</v>
+        <v>0.78319000000000005</v>
       </c>
       <c r="G217">
-        <v>18</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="H217">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="I217" s="57"/>
       <c r="J217" s="51">
         <f t="shared" si="33"/>
-        <v>1.8900000000000583E-3</v>
+        <v>1.2000000000000899E-4</v>
       </c>
       <c r="K217">
         <f t="shared" si="34"/>
-        <v>-8.8000000000000007</v>
+        <v>1</v>
       </c>
       <c r="L217">
         <f t="shared" si="35"/>
-        <v>-1.7000000000000002</v>
+        <v>0.79999999999999982</v>
       </c>
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.2">
@@ -9440,26 +9439,26 @@
         <v>26</v>
       </c>
       <c r="F218" s="51">
-        <v>0.94423999999999997</v>
+        <v>0.93910000000000016</v>
       </c>
       <c r="G218">
-        <v>15</v>
+        <v>7.4</v>
       </c>
       <c r="H218">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="I218" s="57"/>
       <c r="J218" s="51">
         <f t="shared" si="33"/>
-        <v>-2.3639999999999994E-2</v>
+        <v>-1.8500000000000183E-2</v>
       </c>
       <c r="K218">
         <f t="shared" si="34"/>
-        <v>-7.6</v>
+        <v>0</v>
       </c>
       <c r="L218">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>9.9999999999999978E-2</v>
       </c>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.2">
@@ -9479,26 +9478,26 @@
         <v>22</v>
       </c>
       <c r="F219" s="51">
-        <v>0.80137999999999998</v>
+        <v>0.77630999999999994</v>
       </c>
       <c r="G219">
-        <v>13.4</v>
+        <v>6.8</v>
       </c>
       <c r="H219">
-        <v>4.4000000000000004</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I219" s="57"/>
       <c r="J219" s="51">
         <f t="shared" si="33"/>
-        <v>-1.8899999999999917E-2</v>
+        <v>6.1700000000001198E-3</v>
       </c>
       <c r="K219">
         <f t="shared" si="34"/>
-        <v>-6.4</v>
+        <v>0.20000000000000018</v>
       </c>
       <c r="L219">
         <f t="shared" si="35"/>
-        <v>-1.8000000000000003</v>
+        <v>0.39999999999999991</v>
       </c>
     </row>
     <row r="220" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -9518,26 +9517,26 @@
         <v>29</v>
       </c>
       <c r="F220" s="51">
-        <v>0.95601999999999998</v>
+        <v>0.97254000000000007</v>
       </c>
       <c r="G220">
-        <v>17.8</v>
+        <v>9.1</v>
       </c>
       <c r="H220">
-        <v>1.4</v>
+        <v>0.4</v>
       </c>
       <c r="I220" s="57"/>
       <c r="J220" s="55">
         <f t="shared" si="33"/>
-        <v>2.7599999999999847E-3</v>
+        <v>-1.3760000000000105E-2</v>
       </c>
       <c r="K220">
         <f t="shared" si="34"/>
-        <v>-8.9</v>
+        <v>-0.19999999999999929</v>
       </c>
       <c r="L220">
         <f t="shared" si="35"/>
-        <v>-0.49999999999999989</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="221" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
@@ -9546,11 +9545,21 @@
       </c>
       <c r="J221" s="56">
         <f>SUM(J207:J220)</f>
-        <v>0.1199400000000006</v>
+        <v>9.1500000000004356E-3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="E75:H75"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="E56:H56"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="A20:D20"/>
     <mergeCell ref="E96:H96"/>
     <mergeCell ref="A96:D96"/>
     <mergeCell ref="A187:D187"/>
@@ -9565,206 +9574,196 @@
     <mergeCell ref="E151:H151"/>
     <mergeCell ref="A132:D132"/>
     <mergeCell ref="E132:H132"/>
-    <mergeCell ref="E75:H75"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E39:H39"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="E56:H56"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="A20:D20"/>
   </mergeCells>
   <conditionalFormatting sqref="L3:L16">
-    <cfRule type="cellIs" dxfId="99" priority="51" operator="lessThan">
+    <cfRule type="cellIs" dxfId="97" priority="51" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="52" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="96" priority="52" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:K16">
-    <cfRule type="cellIs" dxfId="97" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="95" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="94" priority="50" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41:K54">
-    <cfRule type="cellIs" dxfId="95" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="93" priority="45" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="46" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="92" priority="46" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L41:L54">
-    <cfRule type="cellIs" dxfId="93" priority="47" operator="lessThan">
+    <cfRule type="cellIs" dxfId="91" priority="47" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="48" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J58:K71">
-    <cfRule type="cellIs" dxfId="91" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="89" priority="41" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="42" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L58:L71">
-    <cfRule type="cellIs" dxfId="89" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="87" priority="43" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="44" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J77:K90">
-    <cfRule type="cellIs" dxfId="87" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="85" priority="37" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="84" priority="38" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L77:L90">
-    <cfRule type="cellIs" dxfId="85" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="83" priority="39" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="40" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J98:K111">
-    <cfRule type="cellIs" dxfId="83" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="81" priority="33" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="34" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L98:L111">
-    <cfRule type="cellIs" dxfId="81" priority="35" operator="lessThan">
+    <cfRule type="cellIs" dxfId="79" priority="35" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="36" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J116:K129">
-    <cfRule type="cellIs" dxfId="79" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="77" priority="25" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="26" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L116:L129">
-    <cfRule type="cellIs" dxfId="77" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="75" priority="27" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J134:K147">
-    <cfRule type="cellIs" dxfId="75" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="73" priority="21" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="22" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L134:L147">
-    <cfRule type="cellIs" dxfId="73" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="71" priority="23" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="24" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J153:K166">
-    <cfRule type="cellIs" dxfId="71" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L153:L166">
-    <cfRule type="cellIs" dxfId="69" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="19" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="20" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J171:K184">
-    <cfRule type="cellIs" dxfId="67" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L171:L184">
-    <cfRule type="cellIs" dxfId="65" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="63" priority="15" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J189:K202">
-    <cfRule type="cellIs" dxfId="63" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L189:L202">
-    <cfRule type="cellIs" dxfId="61" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="59" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J207:K220">
-    <cfRule type="cellIs" dxfId="59" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L207:L220">
-    <cfRule type="cellIs" dxfId="57" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="55" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:K35">
-    <cfRule type="cellIs" dxfId="55" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="53" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22:L35">
-    <cfRule type="cellIs" dxfId="53" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="51" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9780,8 +9779,8 @@
   </sheetPr>
   <dimension ref="A1:T144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G149" sqref="G149"/>
+    <sheetView topLeftCell="A106" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="K130" sqref="K130:T143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9793,30 +9792,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="58" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="107" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="108" t="s">
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="108"/>
-      <c r="M1" s="108"/>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="108"/>
-      <c r="S1" s="108"/>
-      <c r="T1" s="108"/>
+      <c r="L1" s="106"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="106"/>
+      <c r="O1" s="106"/>
+      <c r="P1" s="106"/>
+      <c r="Q1" s="106"/>
+      <c r="R1" s="106"/>
+      <c r="S1" s="106"/>
+      <c r="T1" s="106"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -10443,30 +10442,30 @@
       <c r="T12" s="39"/>
     </row>
     <row r="13" spans="1:20" ht="29" x14ac:dyDescent="0.2">
-      <c r="A13" s="102" t="s">
+      <c r="A13" s="107" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="103"/>
-      <c r="C13" s="103"/>
-      <c r="D13" s="103"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="103"/>
-      <c r="G13" s="103"/>
-      <c r="H13" s="103"/>
-      <c r="I13" s="103"/>
-      <c r="J13" s="104"/>
-      <c r="K13" s="105" t="s">
+      <c r="B13" s="108"/>
+      <c r="C13" s="108"/>
+      <c r="D13" s="108"/>
+      <c r="E13" s="108"/>
+      <c r="F13" s="108"/>
+      <c r="G13" s="108"/>
+      <c r="H13" s="108"/>
+      <c r="I13" s="108"/>
+      <c r="J13" s="109"/>
+      <c r="K13" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="L13" s="106"/>
-      <c r="M13" s="106"/>
-      <c r="N13" s="106"/>
-      <c r="O13" s="106"/>
-      <c r="P13" s="106"/>
-      <c r="Q13" s="106"/>
-      <c r="R13" s="106"/>
-      <c r="S13" s="106"/>
-      <c r="T13" s="106"/>
+      <c r="L13" s="104"/>
+      <c r="M13" s="104"/>
+      <c r="N13" s="104"/>
+      <c r="O13" s="104"/>
+      <c r="P13" s="104"/>
+      <c r="Q13" s="104"/>
+      <c r="R13" s="104"/>
+      <c r="S13" s="104"/>
+      <c r="T13" s="104"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="63" t="s">
@@ -11061,30 +11060,30 @@
       <c r="T23" s="39"/>
     </row>
     <row r="25" spans="1:20" ht="29" x14ac:dyDescent="0.2">
-      <c r="A25" s="102" t="s">
+      <c r="A25" s="107" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="103"/>
-      <c r="C25" s="103"/>
-      <c r="D25" s="103"/>
-      <c r="E25" s="103"/>
-      <c r="F25" s="103"/>
-      <c r="G25" s="103"/>
-      <c r="H25" s="103"/>
-      <c r="I25" s="103"/>
-      <c r="J25" s="104"/>
-      <c r="K25" s="105" t="s">
+      <c r="B25" s="108"/>
+      <c r="C25" s="108"/>
+      <c r="D25" s="108"/>
+      <c r="E25" s="108"/>
+      <c r="F25" s="108"/>
+      <c r="G25" s="108"/>
+      <c r="H25" s="108"/>
+      <c r="I25" s="108"/>
+      <c r="J25" s="109"/>
+      <c r="K25" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="L25" s="106"/>
-      <c r="M25" s="106"/>
-      <c r="N25" s="106"/>
-      <c r="O25" s="106"/>
-      <c r="P25" s="106"/>
-      <c r="Q25" s="106"/>
-      <c r="R25" s="106"/>
-      <c r="S25" s="106"/>
-      <c r="T25" s="106"/>
+      <c r="L25" s="104"/>
+      <c r="M25" s="104"/>
+      <c r="N25" s="104"/>
+      <c r="O25" s="104"/>
+      <c r="P25" s="104"/>
+      <c r="Q25" s="104"/>
+      <c r="R25" s="104"/>
+      <c r="S25" s="104"/>
+      <c r="T25" s="104"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
@@ -11667,30 +11666,30 @@
       <c r="T34" s="39"/>
     </row>
     <row r="36" spans="1:20" ht="29" x14ac:dyDescent="0.2">
-      <c r="A36" s="102" t="s">
+      <c r="A36" s="107" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="103"/>
-      <c r="C36" s="103"/>
-      <c r="D36" s="103"/>
-      <c r="E36" s="103"/>
-      <c r="F36" s="103"/>
-      <c r="G36" s="103"/>
-      <c r="H36" s="103"/>
-      <c r="I36" s="103"/>
-      <c r="J36" s="104"/>
-      <c r="K36" s="105" t="s">
+      <c r="B36" s="108"/>
+      <c r="C36" s="108"/>
+      <c r="D36" s="108"/>
+      <c r="E36" s="108"/>
+      <c r="F36" s="108"/>
+      <c r="G36" s="108"/>
+      <c r="H36" s="108"/>
+      <c r="I36" s="108"/>
+      <c r="J36" s="109"/>
+      <c r="K36" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="L36" s="106"/>
-      <c r="M36" s="106"/>
-      <c r="N36" s="106"/>
-      <c r="O36" s="106"/>
-      <c r="P36" s="106"/>
-      <c r="Q36" s="106"/>
-      <c r="R36" s="106"/>
-      <c r="S36" s="106"/>
-      <c r="T36" s="106"/>
+      <c r="L36" s="104"/>
+      <c r="M36" s="104"/>
+      <c r="N36" s="104"/>
+      <c r="O36" s="104"/>
+      <c r="P36" s="104"/>
+      <c r="Q36" s="104"/>
+      <c r="R36" s="104"/>
+      <c r="S36" s="104"/>
+      <c r="T36" s="104"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
@@ -12263,30 +12262,30 @@
       </c>
     </row>
     <row r="47" spans="1:20" ht="29" x14ac:dyDescent="0.2">
-      <c r="A47" s="105" t="s">
+      <c r="A47" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="106"/>
-      <c r="C47" s="106"/>
-      <c r="D47" s="106"/>
-      <c r="E47" s="106"/>
-      <c r="F47" s="106"/>
-      <c r="G47" s="106"/>
-      <c r="H47" s="106"/>
-      <c r="I47" s="106"/>
-      <c r="J47" s="107"/>
-      <c r="K47" s="105" t="s">
+      <c r="B47" s="104"/>
+      <c r="C47" s="104"/>
+      <c r="D47" s="104"/>
+      <c r="E47" s="104"/>
+      <c r="F47" s="104"/>
+      <c r="G47" s="104"/>
+      <c r="H47" s="104"/>
+      <c r="I47" s="104"/>
+      <c r="J47" s="105"/>
+      <c r="K47" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="L47" s="106"/>
-      <c r="M47" s="106"/>
-      <c r="N47" s="106"/>
-      <c r="O47" s="106"/>
-      <c r="P47" s="106"/>
-      <c r="Q47" s="106"/>
-      <c r="R47" s="106"/>
-      <c r="S47" s="106"/>
-      <c r="T47" s="106"/>
+      <c r="L47" s="104"/>
+      <c r="M47" s="104"/>
+      <c r="N47" s="104"/>
+      <c r="O47" s="104"/>
+      <c r="P47" s="104"/>
+      <c r="Q47" s="104"/>
+      <c r="R47" s="104"/>
+      <c r="S47" s="104"/>
+      <c r="T47" s="104"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
@@ -12859,30 +12858,30 @@
       </c>
     </row>
     <row r="58" spans="1:20" ht="29" x14ac:dyDescent="0.2">
-      <c r="A58" s="105" t="s">
+      <c r="A58" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="B58" s="106"/>
-      <c r="C58" s="106"/>
-      <c r="D58" s="106"/>
-      <c r="E58" s="106"/>
-      <c r="F58" s="106"/>
-      <c r="G58" s="106"/>
-      <c r="H58" s="106"/>
-      <c r="I58" s="106"/>
-      <c r="J58" s="107"/>
-      <c r="K58" s="105" t="s">
+      <c r="B58" s="104"/>
+      <c r="C58" s="104"/>
+      <c r="D58" s="104"/>
+      <c r="E58" s="104"/>
+      <c r="F58" s="104"/>
+      <c r="G58" s="104"/>
+      <c r="H58" s="104"/>
+      <c r="I58" s="104"/>
+      <c r="J58" s="105"/>
+      <c r="K58" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="L58" s="106"/>
-      <c r="M58" s="106"/>
-      <c r="N58" s="106"/>
-      <c r="O58" s="106"/>
-      <c r="P58" s="106"/>
-      <c r="Q58" s="106"/>
-      <c r="R58" s="106"/>
-      <c r="S58" s="106"/>
-      <c r="T58" s="106"/>
+      <c r="L58" s="104"/>
+      <c r="M58" s="104"/>
+      <c r="N58" s="104"/>
+      <c r="O58" s="104"/>
+      <c r="P58" s="104"/>
+      <c r="Q58" s="104"/>
+      <c r="R58" s="104"/>
+      <c r="S58" s="104"/>
+      <c r="T58" s="104"/>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="21" t="s">
@@ -13455,30 +13454,30 @@
       </c>
     </row>
     <row r="69" spans="1:20" ht="29" x14ac:dyDescent="0.2">
-      <c r="A69" s="105" t="s">
+      <c r="A69" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="B69" s="106"/>
-      <c r="C69" s="106"/>
-      <c r="D69" s="106"/>
-      <c r="E69" s="106"/>
-      <c r="F69" s="106"/>
-      <c r="G69" s="106"/>
-      <c r="H69" s="106"/>
-      <c r="I69" s="106"/>
-      <c r="J69" s="107"/>
-      <c r="K69" s="105" t="s">
+      <c r="B69" s="104"/>
+      <c r="C69" s="104"/>
+      <c r="D69" s="104"/>
+      <c r="E69" s="104"/>
+      <c r="F69" s="104"/>
+      <c r="G69" s="104"/>
+      <c r="H69" s="104"/>
+      <c r="I69" s="104"/>
+      <c r="J69" s="105"/>
+      <c r="K69" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="L69" s="106"/>
-      <c r="M69" s="106"/>
-      <c r="N69" s="106"/>
-      <c r="O69" s="106"/>
-      <c r="P69" s="106"/>
-      <c r="Q69" s="106"/>
-      <c r="R69" s="106"/>
-      <c r="S69" s="106"/>
-      <c r="T69" s="106"/>
+      <c r="L69" s="104"/>
+      <c r="M69" s="104"/>
+      <c r="N69" s="104"/>
+      <c r="O69" s="104"/>
+      <c r="P69" s="104"/>
+      <c r="Q69" s="104"/>
+      <c r="R69" s="104"/>
+      <c r="S69" s="104"/>
+      <c r="T69" s="104"/>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70" s="44" t="s">
@@ -14051,30 +14050,30 @@
       </c>
     </row>
     <row r="82" spans="1:20" ht="29" x14ac:dyDescent="0.2">
-      <c r="A82" s="105" t="s">
+      <c r="A82" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="B82" s="106"/>
-      <c r="C82" s="106"/>
-      <c r="D82" s="106"/>
-      <c r="E82" s="106"/>
-      <c r="F82" s="106"/>
-      <c r="G82" s="106"/>
-      <c r="H82" s="106"/>
-      <c r="I82" s="106"/>
-      <c r="J82" s="107"/>
-      <c r="K82" s="105" t="s">
+      <c r="B82" s="104"/>
+      <c r="C82" s="104"/>
+      <c r="D82" s="104"/>
+      <c r="E82" s="104"/>
+      <c r="F82" s="104"/>
+      <c r="G82" s="104"/>
+      <c r="H82" s="104"/>
+      <c r="I82" s="104"/>
+      <c r="J82" s="105"/>
+      <c r="K82" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="L82" s="106"/>
-      <c r="M82" s="106"/>
-      <c r="N82" s="106"/>
-      <c r="O82" s="106"/>
-      <c r="P82" s="106"/>
-      <c r="Q82" s="106"/>
-      <c r="R82" s="106"/>
-      <c r="S82" s="106"/>
-      <c r="T82" s="106"/>
+      <c r="L82" s="104"/>
+      <c r="M82" s="104"/>
+      <c r="N82" s="104"/>
+      <c r="O82" s="104"/>
+      <c r="P82" s="104"/>
+      <c r="Q82" s="104"/>
+      <c r="R82" s="104"/>
+      <c r="S82" s="104"/>
+      <c r="T82" s="104"/>
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83" s="44" t="s">
@@ -14647,30 +14646,30 @@
       </c>
     </row>
     <row r="94" spans="1:20" ht="29" x14ac:dyDescent="0.2">
-      <c r="A94" s="105" t="s">
+      <c r="A94" s="103" t="s">
         <v>52</v>
       </c>
-      <c r="B94" s="106"/>
-      <c r="C94" s="106"/>
-      <c r="D94" s="106"/>
-      <c r="E94" s="106"/>
-      <c r="F94" s="106"/>
-      <c r="G94" s="106"/>
-      <c r="H94" s="106"/>
-      <c r="I94" s="106"/>
-      <c r="J94" s="107"/>
-      <c r="K94" s="105" t="s">
+      <c r="B94" s="104"/>
+      <c r="C94" s="104"/>
+      <c r="D94" s="104"/>
+      <c r="E94" s="104"/>
+      <c r="F94" s="104"/>
+      <c r="G94" s="104"/>
+      <c r="H94" s="104"/>
+      <c r="I94" s="104"/>
+      <c r="J94" s="105"/>
+      <c r="K94" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="L94" s="106"/>
-      <c r="M94" s="106"/>
-      <c r="N94" s="106"/>
-      <c r="O94" s="106"/>
-      <c r="P94" s="106"/>
-      <c r="Q94" s="106"/>
-      <c r="R94" s="106"/>
-      <c r="S94" s="106"/>
-      <c r="T94" s="106"/>
+      <c r="L94" s="104"/>
+      <c r="M94" s="104"/>
+      <c r="N94" s="104"/>
+      <c r="O94" s="104"/>
+      <c r="P94" s="104"/>
+      <c r="Q94" s="104"/>
+      <c r="R94" s="104"/>
+      <c r="S94" s="104"/>
+      <c r="T94" s="104"/>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
@@ -15243,30 +15242,30 @@
       </c>
     </row>
     <row r="106" spans="1:20" ht="29" x14ac:dyDescent="0.2">
-      <c r="A106" s="102" t="s">
+      <c r="A106" s="107" t="s">
         <v>54</v>
       </c>
-      <c r="B106" s="103"/>
-      <c r="C106" s="103"/>
-      <c r="D106" s="103"/>
-      <c r="E106" s="103"/>
-      <c r="F106" s="103"/>
-      <c r="G106" s="103"/>
-      <c r="H106" s="103"/>
-      <c r="I106" s="103"/>
-      <c r="J106" s="104"/>
-      <c r="K106" s="105" t="s">
+      <c r="B106" s="108"/>
+      <c r="C106" s="108"/>
+      <c r="D106" s="108"/>
+      <c r="E106" s="108"/>
+      <c r="F106" s="108"/>
+      <c r="G106" s="108"/>
+      <c r="H106" s="108"/>
+      <c r="I106" s="108"/>
+      <c r="J106" s="109"/>
+      <c r="K106" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="L106" s="106"/>
-      <c r="M106" s="106"/>
-      <c r="N106" s="106"/>
-      <c r="O106" s="106"/>
-      <c r="P106" s="106"/>
-      <c r="Q106" s="106"/>
-      <c r="R106" s="106"/>
-      <c r="S106" s="106"/>
-      <c r="T106" s="106"/>
+      <c r="L106" s="104"/>
+      <c r="M106" s="104"/>
+      <c r="N106" s="104"/>
+      <c r="O106" s="104"/>
+      <c r="P106" s="104"/>
+      <c r="Q106" s="104"/>
+      <c r="R106" s="104"/>
+      <c r="S106" s="104"/>
+      <c r="T106" s="104"/>
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A107" s="59" t="s">
@@ -15839,30 +15838,30 @@
       </c>
     </row>
     <row r="118" spans="1:20" ht="29" x14ac:dyDescent="0.2">
-      <c r="A118" s="102" t="s">
+      <c r="A118" s="107" t="s">
         <v>56</v>
       </c>
-      <c r="B118" s="103"/>
-      <c r="C118" s="103"/>
-      <c r="D118" s="103"/>
-      <c r="E118" s="103"/>
-      <c r="F118" s="103"/>
-      <c r="G118" s="103"/>
-      <c r="H118" s="103"/>
-      <c r="I118" s="103"/>
-      <c r="J118" s="104"/>
-      <c r="K118" s="105" t="s">
+      <c r="B118" s="108"/>
+      <c r="C118" s="108"/>
+      <c r="D118" s="108"/>
+      <c r="E118" s="108"/>
+      <c r="F118" s="108"/>
+      <c r="G118" s="108"/>
+      <c r="H118" s="108"/>
+      <c r="I118" s="108"/>
+      <c r="J118" s="109"/>
+      <c r="K118" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="L118" s="106"/>
-      <c r="M118" s="106"/>
-      <c r="N118" s="106"/>
-      <c r="O118" s="106"/>
-      <c r="P118" s="106"/>
-      <c r="Q118" s="106"/>
-      <c r="R118" s="106"/>
-      <c r="S118" s="106"/>
-      <c r="T118" s="106"/>
+      <c r="L118" s="104"/>
+      <c r="M118" s="104"/>
+      <c r="N118" s="104"/>
+      <c r="O118" s="104"/>
+      <c r="P118" s="104"/>
+      <c r="Q118" s="104"/>
+      <c r="R118" s="104"/>
+      <c r="S118" s="104"/>
+      <c r="T118" s="104"/>
     </row>
     <row r="119" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
@@ -16435,30 +16434,30 @@
       </c>
     </row>
     <row r="130" spans="1:20" ht="29" x14ac:dyDescent="0.2">
-      <c r="A130" s="102" t="s">
+      <c r="A130" s="107" t="s">
         <v>63</v>
       </c>
-      <c r="B130" s="103"/>
-      <c r="C130" s="103"/>
-      <c r="D130" s="103"/>
-      <c r="E130" s="103"/>
-      <c r="F130" s="103"/>
-      <c r="G130" s="103"/>
-      <c r="H130" s="103"/>
-      <c r="I130" s="103"/>
-      <c r="J130" s="104"/>
-      <c r="K130" s="105" t="s">
+      <c r="B130" s="108"/>
+      <c r="C130" s="108"/>
+      <c r="D130" s="108"/>
+      <c r="E130" s="108"/>
+      <c r="F130" s="108"/>
+      <c r="G130" s="108"/>
+      <c r="H130" s="108"/>
+      <c r="I130" s="108"/>
+      <c r="J130" s="109"/>
+      <c r="K130" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="L130" s="106"/>
-      <c r="M130" s="106"/>
-      <c r="N130" s="106"/>
-      <c r="O130" s="106"/>
-      <c r="P130" s="106"/>
-      <c r="Q130" s="106"/>
-      <c r="R130" s="106"/>
-      <c r="S130" s="106"/>
-      <c r="T130" s="106"/>
+      <c r="L130" s="104"/>
+      <c r="M130" s="104"/>
+      <c r="N130" s="104"/>
+      <c r="O130" s="104"/>
+      <c r="P130" s="104"/>
+      <c r="Q130" s="104"/>
+      <c r="R130" s="104"/>
+      <c r="S130" s="104"/>
+      <c r="T130" s="104"/>
     </row>
     <row r="131" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
@@ -16987,7 +16986,7 @@
       <c r="J139" s="70">
         <v>0.88706300000000005</v>
       </c>
-      <c r="K139" s="110" t="s">
+      <c r="K139" s="98" t="s">
         <v>61</v>
       </c>
       <c r="L139" s="5">
@@ -17049,7 +17048,7 @@
       <c r="J140" s="70">
         <v>0.89604200000000001</v>
       </c>
-      <c r="K140" s="110" t="s">
+      <c r="K140" s="98" t="s">
         <v>62</v>
       </c>
       <c r="L140" s="5">
@@ -17111,7 +17110,7 @@
       <c r="J141" s="74">
         <v>0.905003</v>
       </c>
-      <c r="K141" s="110" t="s">
+      <c r="K141" s="98" t="s">
         <v>58</v>
       </c>
       <c r="L141" s="5">
@@ -17342,6 +17341,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A118:J118"/>
+    <mergeCell ref="K118:T118"/>
+    <mergeCell ref="A130:J130"/>
+    <mergeCell ref="K130:T130"/>
+    <mergeCell ref="A69:J69"/>
+    <mergeCell ref="K69:T69"/>
+    <mergeCell ref="A106:J106"/>
+    <mergeCell ref="K106:T106"/>
+    <mergeCell ref="A94:J94"/>
+    <mergeCell ref="K94:T94"/>
+    <mergeCell ref="K82:T82"/>
+    <mergeCell ref="A82:J82"/>
     <mergeCell ref="A58:J58"/>
     <mergeCell ref="K58:T58"/>
     <mergeCell ref="K47:T47"/>
@@ -17354,206 +17365,194 @@
     <mergeCell ref="K36:T36"/>
     <mergeCell ref="K13:T13"/>
     <mergeCell ref="A13:J13"/>
-    <mergeCell ref="A118:J118"/>
-    <mergeCell ref="K118:T118"/>
-    <mergeCell ref="A130:J130"/>
-    <mergeCell ref="K130:T130"/>
-    <mergeCell ref="A69:J69"/>
-    <mergeCell ref="K69:T69"/>
-    <mergeCell ref="A106:J106"/>
-    <mergeCell ref="K106:T106"/>
-    <mergeCell ref="A94:J94"/>
-    <mergeCell ref="K94:T94"/>
-    <mergeCell ref="K82:T82"/>
-    <mergeCell ref="A82:J82"/>
   </mergeCells>
   <conditionalFormatting sqref="C34:F34 I34:J34">
-    <cfRule type="cellIs" dxfId="51" priority="62" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="62" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:F34 I34:J34">
-    <cfRule type="cellIs" dxfId="50" priority="61" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="61" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34:H34">
-    <cfRule type="cellIs" dxfId="49" priority="53" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="53" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="54" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:F12 I10:J12 I23:J23 C23:F23">
-    <cfRule type="cellIs" dxfId="47" priority="52" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="52" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:F12 I10:J12 I23:J23 C23:F23">
-    <cfRule type="cellIs" dxfId="46" priority="51" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="51" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:H12 G23:H23">
-    <cfRule type="cellIs" dxfId="45" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="50" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:F45 I45:J45">
-    <cfRule type="cellIs" dxfId="43" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="48" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:F45 I45:J45">
-    <cfRule type="cellIs" dxfId="42" priority="47" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="47" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45:H45">
-    <cfRule type="cellIs" dxfId="41" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="45" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="46" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="46" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:F56 I56:J56">
-    <cfRule type="cellIs" dxfId="39" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="44" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:F56 I56:J56">
-    <cfRule type="cellIs" dxfId="38" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="43" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56:H56">
-    <cfRule type="cellIs" dxfId="37" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="35" priority="41" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="42" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67:F67 I67:J67">
-    <cfRule type="cellIs" dxfId="35" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="40" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67:F67 I67:J67">
-    <cfRule type="cellIs" dxfId="34" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="39" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G67:H67">
-    <cfRule type="cellIs" dxfId="33" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="37" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="38" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C78:F78 I78:J78">
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="32" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C78:F78 I78:J78">
-    <cfRule type="cellIs" dxfId="30" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="31" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G78:H78">
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91:F91 I91:J91">
-    <cfRule type="cellIs" dxfId="27" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91:F91 I91:J91">
-    <cfRule type="cellIs" dxfId="26" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G91:H91">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103:F103 I103:J103">
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103:F103 I103:J103">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="23" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G103:H103">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C115:F115 I115:J115">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C115:F115 I115:J115">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G115:H115">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C127:F127 I127:J127">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C127:F127 I127:J127">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G127:H127">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C144:E144 I144:J144">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C144:E144 I144:J144">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17600,10 +17599,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDF478C-84F8-7949-9002-5ABF95255D36}">
-  <dimension ref="B2:AH49"/>
+  <dimension ref="B2:AH66"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="T1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="AH48" sqref="AH48"/>
+    <sheetView showGridLines="0" topLeftCell="L1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="Y68" sqref="Y68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17622,26 +17621,26 @@
   <sheetData>
     <row r="2" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="84"/>
-      <c r="C2" s="109" t="s">
+      <c r="C2" s="110" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
       <c r="J2" s="85"/>
       <c r="N2" s="84"/>
-      <c r="O2" s="109" t="s">
+      <c r="O2" s="110" t="s">
         <v>71</v>
       </c>
-      <c r="P2" s="109"/>
-      <c r="Q2" s="109"/>
-      <c r="R2" s="109"/>
-      <c r="S2" s="109"/>
-      <c r="T2" s="109"/>
-      <c r="U2" s="109"/>
+      <c r="P2" s="110"/>
+      <c r="Q2" s="110"/>
+      <c r="R2" s="110"/>
+      <c r="S2" s="110"/>
+      <c r="T2" s="110"/>
+      <c r="U2" s="110"/>
       <c r="V2" s="85"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.2">
@@ -17740,7 +17739,7 @@
       <c r="J5" s="87"/>
       <c r="N5" s="86"/>
       <c r="O5" s="42" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="P5" s="5">
         <f>Overall!C44</f>
@@ -17771,7 +17770,7 @@
     <row r="6" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B6" s="86"/>
       <c r="C6" s="42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D6" s="5">
         <f>Overall!M33</f>
@@ -17800,7 +17799,7 @@
       <c r="J6" s="87"/>
       <c r="N6" s="86"/>
       <c r="O6" s="42" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="P6" s="5">
         <f>Overall!C114</f>
@@ -17840,7 +17839,7 @@
       <c r="J7" s="91"/>
       <c r="N7" s="86"/>
       <c r="O7" s="42" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P7" s="5">
         <v>0.79</v>
@@ -17875,26 +17874,26 @@
     </row>
     <row r="10" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="84"/>
-      <c r="C10" s="109" t="s">
+      <c r="C10" s="110" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="109"/>
-      <c r="E10" s="109"/>
-      <c r="F10" s="109"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="109"/>
-      <c r="I10" s="109"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="110"/>
+      <c r="H10" s="110"/>
+      <c r="I10" s="110"/>
       <c r="J10" s="85"/>
       <c r="N10" s="84"/>
-      <c r="O10" s="109" t="s">
-        <v>77</v>
-      </c>
-      <c r="P10" s="109"/>
-      <c r="Q10" s="109"/>
-      <c r="R10" s="109"/>
-      <c r="S10" s="109"/>
-      <c r="T10" s="109"/>
-      <c r="U10" s="109"/>
+      <c r="O10" s="110" t="s">
+        <v>75</v>
+      </c>
+      <c r="P10" s="110"/>
+      <c r="Q10" s="110"/>
+      <c r="R10" s="110"/>
+      <c r="S10" s="110"/>
+      <c r="T10" s="110"/>
+      <c r="U10" s="110"/>
       <c r="V10" s="85"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.2">
@@ -17993,7 +17992,7 @@
       <c r="J13" s="87"/>
       <c r="N13" s="86"/>
       <c r="O13" s="42" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P13" s="5">
         <f>Overall!C77</f>
@@ -18024,7 +18023,7 @@
     <row r="14" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B14" s="86"/>
       <c r="C14" s="92" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D14" s="5">
         <f>Overall!M21</f>
@@ -18053,7 +18052,7 @@
       <c r="J14" s="87"/>
       <c r="N14" s="86"/>
       <c r="O14" s="42" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P14" s="5">
         <f>Overall!C126</f>
@@ -18113,7 +18112,7 @@
       <c r="J15" s="87"/>
       <c r="N15" s="86"/>
       <c r="O15" s="42" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P15" s="5">
         <v>0.79</v>
@@ -18157,15 +18156,15 @@
     </row>
     <row r="19" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="84"/>
-      <c r="C19" s="109" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="109"/>
-      <c r="E19" s="109"/>
-      <c r="F19" s="109"/>
-      <c r="G19" s="109"/>
-      <c r="H19" s="109"/>
-      <c r="I19" s="109"/>
+      <c r="C19" s="110" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="110"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="110"/>
+      <c r="G19" s="110"/>
+      <c r="H19" s="110"/>
+      <c r="I19" s="110"/>
       <c r="J19" s="85"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
@@ -18205,7 +18204,7 @@
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="86"/>
       <c r="C22" s="42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D22" s="5">
         <f>Overall!C66</f>
@@ -18236,7 +18235,7 @@
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="86"/>
       <c r="C23" s="42" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D23" s="5">
         <v>0.79</v>
@@ -18274,15 +18273,15 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" s="84"/>
-      <c r="C27" s="109" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="109"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="109"/>
-      <c r="G27" s="109"/>
-      <c r="H27" s="109"/>
-      <c r="I27" s="109"/>
+      <c r="C27" s="110" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="110"/>
+      <c r="E27" s="110"/>
+      <c r="F27" s="110"/>
+      <c r="G27" s="110"/>
+      <c r="H27" s="110"/>
+      <c r="I27" s="110"/>
       <c r="J27" s="85"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
@@ -18322,7 +18321,7 @@
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B30" s="86"/>
       <c r="C30" s="92" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D30" s="5">
         <v>0.79</v>
@@ -18418,18 +18417,18 @@
       <c r="J33" s="91"/>
     </row>
     <row r="36" spans="2:34" ht="29" x14ac:dyDescent="0.2">
-      <c r="Y36" s="102" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z36" s="103"/>
-      <c r="AA36" s="103"/>
-      <c r="AB36" s="103"/>
-      <c r="AC36" s="103"/>
-      <c r="AD36" s="103"/>
-      <c r="AE36" s="103"/>
-      <c r="AF36" s="103"/>
-      <c r="AG36" s="103"/>
-      <c r="AH36" s="105"/>
+      <c r="Y36" s="107" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z36" s="108"/>
+      <c r="AA36" s="108"/>
+      <c r="AB36" s="108"/>
+      <c r="AC36" s="108"/>
+      <c r="AD36" s="108"/>
+      <c r="AE36" s="108"/>
+      <c r="AF36" s="108"/>
+      <c r="AG36" s="108"/>
+      <c r="AH36" s="103"/>
     </row>
     <row r="37" spans="2:34" x14ac:dyDescent="0.2">
       <c r="Y37" s="1" t="s">
@@ -18865,8 +18864,457 @@
         <v>0.89326100000000008</v>
       </c>
     </row>
+    <row r="53" spans="25:34" ht="29" x14ac:dyDescent="0.2">
+      <c r="Y53" s="104" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z53" s="104"/>
+      <c r="AA53" s="104"/>
+      <c r="AB53" s="104"/>
+      <c r="AC53" s="104"/>
+      <c r="AD53" s="104"/>
+      <c r="AE53" s="104"/>
+      <c r="AF53" s="104"/>
+      <c r="AG53" s="104"/>
+      <c r="AH53" s="104"/>
+    </row>
+    <row r="54" spans="25:34" x14ac:dyDescent="0.2">
+      <c r="Y54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH54" s="35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="25:34" x14ac:dyDescent="0.2">
+      <c r="Y55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z55" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="AA55" s="5">
+        <v>0.79</v>
+      </c>
+      <c r="AB55" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="AC55" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="AD55" s="5">
+        <v>107</v>
+      </c>
+      <c r="AE55" s="5">
+        <v>28</v>
+      </c>
+      <c r="AF55" s="5">
+        <v>26</v>
+      </c>
+      <c r="AG55" s="5">
+        <v>0.59209999999999996</v>
+      </c>
+      <c r="AH55" s="58">
+        <v>0.85262099999999996</v>
+      </c>
+    </row>
+    <row r="56" spans="25:34" x14ac:dyDescent="0.2">
+      <c r="Y56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z56" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="AA56" s="5">
+        <v>0.79</v>
+      </c>
+      <c r="AB56" s="5">
+        <v>0.88</v>
+      </c>
+      <c r="AC56" s="5">
+        <v>0.83</v>
+      </c>
+      <c r="AD56" s="5">
+        <v>112</v>
+      </c>
+      <c r="AE56" s="5">
+        <v>29</v>
+      </c>
+      <c r="AF56" s="5">
+        <v>16</v>
+      </c>
+      <c r="AG56" s="5">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="AH56" s="58">
+        <v>0.91647000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="25:34" x14ac:dyDescent="0.2">
+      <c r="Y57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z57" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="AA57" s="5">
+        <v>0.78</v>
+      </c>
+      <c r="AB57" s="5">
+        <v>0.76</v>
+      </c>
+      <c r="AC57" s="5">
+        <v>0.77</v>
+      </c>
+      <c r="AD57" s="5">
+        <v>98</v>
+      </c>
+      <c r="AE57" s="5">
+        <v>27</v>
+      </c>
+      <c r="AF57" s="5">
+        <v>31</v>
+      </c>
+      <c r="AG57" s="5">
+        <v>0.59770000000000001</v>
+      </c>
+      <c r="AH57" s="58">
+        <v>0.86721700000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="25:34" x14ac:dyDescent="0.2">
+      <c r="Y58" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z58" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="AA58" s="5">
+        <v>0.84</v>
+      </c>
+      <c r="AB58" s="5">
+        <v>0.85</v>
+      </c>
+      <c r="AC58" s="5">
+        <v>0.84</v>
+      </c>
+      <c r="AD58" s="5">
+        <v>111</v>
+      </c>
+      <c r="AE58" s="5">
+        <v>21</v>
+      </c>
+      <c r="AF58" s="5">
+        <v>20</v>
+      </c>
+      <c r="AG58" s="5">
+        <v>0.6321</v>
+      </c>
+      <c r="AH58" s="58">
+        <v>0.93681199999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="25:34" x14ac:dyDescent="0.2">
+      <c r="Y59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z59" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="AA59" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="AB59" s="5">
+        <v>0.83</v>
+      </c>
+      <c r="AC59" s="5">
+        <v>0.81</v>
+      </c>
+      <c r="AD59" s="5">
+        <v>109</v>
+      </c>
+      <c r="AE59" s="5">
+        <v>27</v>
+      </c>
+      <c r="AF59" s="5">
+        <v>23</v>
+      </c>
+      <c r="AG59" s="5">
+        <v>0.61009999999999998</v>
+      </c>
+      <c r="AH59" s="58">
+        <v>0.88785999999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="25:34" x14ac:dyDescent="0.2">
+      <c r="Y60" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z60" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="AA60" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="AB60" s="5">
+        <v>0.83</v>
+      </c>
+      <c r="AC60" s="5">
+        <v>0.81</v>
+      </c>
+      <c r="AD60" s="5">
+        <v>109</v>
+      </c>
+      <c r="AE60" s="5">
+        <v>28</v>
+      </c>
+      <c r="AF60" s="5">
+        <v>22</v>
+      </c>
+      <c r="AG60" s="5">
+        <v>0.59279999999999999</v>
+      </c>
+      <c r="AH60" s="82">
+        <v>0.90634199999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="25:34" x14ac:dyDescent="0.2">
+      <c r="Y61" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z61" s="42">
+        <v>0.25</v>
+      </c>
+      <c r="AA61" s="42">
+        <v>0.79</v>
+      </c>
+      <c r="AB61" s="71">
+        <v>0.79</v>
+      </c>
+      <c r="AC61" s="42">
+        <v>0.79</v>
+      </c>
+      <c r="AD61" s="42">
+        <v>110</v>
+      </c>
+      <c r="AE61" s="42">
+        <v>30</v>
+      </c>
+      <c r="AF61" s="42">
+        <v>29</v>
+      </c>
+      <c r="AG61" s="42">
+        <v>0.60140000000000005</v>
+      </c>
+      <c r="AH61" s="113">
+        <v>0.88501300000000005</v>
+      </c>
+    </row>
+    <row r="62" spans="25:34" x14ac:dyDescent="0.2">
+      <c r="Y62" s="111" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z62" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="AA62" s="5">
+        <v>0.82</v>
+      </c>
+      <c r="AB62" s="5">
+        <v>0.82</v>
+      </c>
+      <c r="AC62" s="5">
+        <v>0.82</v>
+      </c>
+      <c r="AD62" s="5">
+        <v>107</v>
+      </c>
+      <c r="AE62" s="5">
+        <v>24</v>
+      </c>
+      <c r="AF62" s="5">
+        <v>23</v>
+      </c>
+      <c r="AG62" s="5">
+        <v>0.62849999999999995</v>
+      </c>
+      <c r="AH62" s="58">
+        <v>0.88811799999999996</v>
+      </c>
+    </row>
+    <row r="63" spans="25:34" x14ac:dyDescent="0.2">
+      <c r="Y63" s="111" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z63" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="AA63" s="5">
+        <v>0.76</v>
+      </c>
+      <c r="AB63" s="5">
+        <v>0.82</v>
+      </c>
+      <c r="AC63" s="5">
+        <v>0.79</v>
+      </c>
+      <c r="AD63" s="5">
+        <v>108</v>
+      </c>
+      <c r="AE63" s="5">
+        <v>35</v>
+      </c>
+      <c r="AF63" s="5">
+        <v>24</v>
+      </c>
+      <c r="AG63" s="5">
+        <v>0.56740000000000002</v>
+      </c>
+      <c r="AH63" s="58">
+        <v>0.88479699999999994</v>
+      </c>
+    </row>
+    <row r="64" spans="25:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y64" s="112" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z64" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="AA64" s="12">
+        <v>0.79</v>
+      </c>
+      <c r="AB64" s="12">
+        <v>0.77</v>
+      </c>
+      <c r="AC64" s="12">
+        <v>0.78</v>
+      </c>
+      <c r="AD64" s="12">
+        <v>99</v>
+      </c>
+      <c r="AE64" s="12">
+        <v>27</v>
+      </c>
+      <c r="AF64" s="12">
+        <v>30</v>
+      </c>
+      <c r="AG64" s="12">
+        <v>0.59219999999999995</v>
+      </c>
+      <c r="AH64" s="95">
+        <v>0.89947699999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="25:34" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="Y65" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z65" s="15">
+        <f t="shared" ref="Z65:AG65" si="2">STDEV(Z55:Z64)</f>
+        <v>0</v>
+      </c>
+      <c r="AA65" s="96">
+        <f t="shared" si="2"/>
+        <v>2.1705094128132922E-2</v>
+      </c>
+      <c r="AB65" s="96">
+        <f t="shared" si="2"/>
+        <v>3.6285901761795386E-2</v>
+      </c>
+      <c r="AC65" s="96">
+        <f t="shared" si="2"/>
+        <v>2.2211108331943553E-2</v>
+      </c>
+      <c r="AD65" s="96">
+        <f t="shared" si="2"/>
+        <v>4.7609522856952333</v>
+      </c>
+      <c r="AE65" s="96">
+        <f t="shared" si="2"/>
+        <v>3.657564459825382</v>
+      </c>
+      <c r="AF65" s="96">
+        <f t="shared" si="2"/>
+        <v>4.695151163109065</v>
+      </c>
+      <c r="AG65" s="96">
+        <f t="shared" si="2"/>
+        <v>1.8904676082328879E-2</v>
+      </c>
+      <c r="AH65" s="97">
+        <f>STDEV(AH55:AH64)</f>
+        <v>2.3953830396781593E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="25:34" x14ac:dyDescent="0.2">
+      <c r="Y66" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z66" s="42">
+        <f>MEDIAN(Z55:Z64)</f>
+        <v>0.25</v>
+      </c>
+      <c r="AA66" s="42">
+        <f t="shared" ref="AA66:AH66" si="3">MEDIAN(AA55:AA64)</f>
+        <v>0.79</v>
+      </c>
+      <c r="AB66" s="42">
+        <f t="shared" si="3"/>
+        <v>0.82</v>
+      </c>
+      <c r="AC66" s="42">
+        <f t="shared" si="3"/>
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="AD66" s="42">
+        <f t="shared" si="3"/>
+        <v>108.5</v>
+      </c>
+      <c r="AE66" s="42">
+        <f t="shared" si="3"/>
+        <v>27.5</v>
+      </c>
+      <c r="AF66" s="42">
+        <f t="shared" si="3"/>
+        <v>23.5</v>
+      </c>
+      <c r="AG66" s="42">
+        <f t="shared" si="3"/>
+        <v>0.59955000000000003</v>
+      </c>
+      <c r="AH66" s="72">
+        <f t="shared" si="3"/>
+        <v>0.88798899999999992</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="Y53:AH53"/>
     <mergeCell ref="C27:I27"/>
     <mergeCell ref="O10:U10"/>
     <mergeCell ref="Y36:AH36"/>

</xml_diff>